<commit_message>
feat(publipostage): Add new indicator about 10 years and Drug
and list of all indicators of all sponsors
</commit_message>
<xml_diff>
--- a/publipostage/002cp4060/liste_essais_cliniques_identifies_002cp4060.xlsx
+++ b/publipostage/002cp4060/liste_essais_cliniques_identifies_002cp4060.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J214"/>
+  <dimension ref="A1:K214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>results</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>intervention_type</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -522,6 +527,11 @@
       <c r="J2" t="b">
         <v>1</v>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -560,6 +570,11 @@
       <c r="J3" t="b">
         <v>0</v>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -602,6 +617,11 @@
       <c r="J4" t="b">
         <v>0</v>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -640,6 +660,11 @@
       <c r="J5" t="b">
         <v>0</v>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -678,6 +703,11 @@
       <c r="J6" t="b">
         <v>1</v>
       </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -716,6 +746,11 @@
       <c r="J7" t="b">
         <v>0</v>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -754,6 +789,11 @@
       <c r="J8" t="b">
         <v>0</v>
       </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -792,6 +832,11 @@
       <c r="J9" t="b">
         <v>0</v>
       </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -830,6 +875,11 @@
       <c r="J10" t="b">
         <v>0</v>
       </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -868,6 +918,11 @@
       <c r="J11" t="b">
         <v>0</v>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -906,6 +961,11 @@
       <c r="J12" t="b">
         <v>0</v>
       </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -944,6 +1004,11 @@
       <c r="J13" t="b">
         <v>0</v>
       </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -982,6 +1047,11 @@
       <c r="J14" t="b">
         <v>1</v>
       </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1020,6 +1090,11 @@
       <c r="J15" t="b">
         <v>0</v>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1058,6 +1133,11 @@
       <c r="J16" t="b">
         <v>1</v>
       </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>DIETARY_SUPPLEMENT</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1100,6 +1180,11 @@
       <c r="J17" t="b">
         <v>1</v>
       </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1138,6 +1223,11 @@
       <c r="J18" t="b">
         <v>0</v>
       </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1176,6 +1266,11 @@
       <c r="J19" t="b">
         <v>0</v>
       </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1214,6 +1309,11 @@
       <c r="J20" t="b">
         <v>0</v>
       </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1252,6 +1352,11 @@
       <c r="J21" t="b">
         <v>0</v>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1289,6 +1394,11 @@
       </c>
       <c r="J22" t="b">
         <v>0</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1324,6 +1434,11 @@
       <c r="J23" t="b">
         <v>0</v>
       </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1358,6 +1473,11 @@
       <c r="J24" t="b">
         <v>0</v>
       </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1396,6 +1516,11 @@
       <c r="J25" t="b">
         <v>1</v>
       </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1434,6 +1559,11 @@
       <c r="J26" t="b">
         <v>0</v>
       </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1472,6 +1602,11 @@
       <c r="J27" t="b">
         <v>0</v>
       </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1510,6 +1645,11 @@
       <c r="J28" t="b">
         <v>0</v>
       </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1548,6 +1688,11 @@
       <c r="J29" t="b">
         <v>0</v>
       </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1586,6 +1731,11 @@
       <c r="J30" t="b">
         <v>0</v>
       </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1624,6 +1774,11 @@
       <c r="J31" t="b">
         <v>0</v>
       </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1661,6 +1816,11 @@
       </c>
       <c r="J32" t="b">
         <v>1</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1696,6 +1856,11 @@
       <c r="J33" t="b">
         <v>1</v>
       </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1734,6 +1899,11 @@
       <c r="J34" t="b">
         <v>0</v>
       </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1771,6 +1941,11 @@
       </c>
       <c r="J35" t="b">
         <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1806,6 +1981,11 @@
       <c r="J36" t="b">
         <v>1</v>
       </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1844,6 +2024,11 @@
       <c r="J37" t="b">
         <v>0</v>
       </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1882,6 +2067,11 @@
       <c r="J38" t="b">
         <v>0</v>
       </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1920,6 +2110,11 @@
       <c r="J39" t="b">
         <v>0</v>
       </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1958,6 +2153,11 @@
       <c r="J40" t="b">
         <v>0</v>
       </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1996,6 +2196,11 @@
       <c r="J41" t="b">
         <v>1</v>
       </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2034,6 +2239,11 @@
       <c r="J42" t="b">
         <v>0</v>
       </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2072,6 +2282,11 @@
       <c r="J43" t="b">
         <v>0</v>
       </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2110,6 +2325,11 @@
       <c r="J44" t="b">
         <v>0</v>
       </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2152,6 +2372,11 @@
       <c r="J45" t="b">
         <v>0</v>
       </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2190,6 +2415,11 @@
       <c r="J46" t="b">
         <v>0</v>
       </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2228,6 +2458,11 @@
       <c r="J47" t="b">
         <v>1</v>
       </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2266,6 +2501,11 @@
       <c r="J48" t="b">
         <v>0</v>
       </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>DIETARY_SUPPLEMENT</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2304,6 +2544,11 @@
       <c r="J49" t="b">
         <v>0</v>
       </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2346,6 +2591,11 @@
       <c r="J50" t="b">
         <v>1</v>
       </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2384,6 +2634,11 @@
       <c r="J51" t="b">
         <v>0</v>
       </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2422,6 +2677,11 @@
       <c r="J52" t="b">
         <v>0</v>
       </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2460,6 +2720,11 @@
       <c r="J53" t="b">
         <v>0</v>
       </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2498,6 +2763,11 @@
       <c r="J54" t="b">
         <v>0</v>
       </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2536,6 +2806,11 @@
       <c r="J55" t="b">
         <v>0</v>
       </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2574,6 +2849,11 @@
       <c r="J56" t="b">
         <v>0</v>
       </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>GENETIC</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2612,6 +2892,11 @@
       <c r="J57" t="b">
         <v>0</v>
       </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>GENETIC</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2650,6 +2935,11 @@
       <c r="J58" t="b">
         <v>0</v>
       </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2688,6 +2978,11 @@
       <c r="J59" t="b">
         <v>0</v>
       </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>GENETIC</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2726,6 +3021,11 @@
       <c r="J60" t="b">
         <v>0</v>
       </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2768,6 +3068,11 @@
       <c r="J61" t="b">
         <v>1</v>
       </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2806,6 +3111,11 @@
       <c r="J62" t="b">
         <v>0</v>
       </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2844,6 +3154,11 @@
       <c r="J63" t="b">
         <v>0</v>
       </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2882,6 +3197,11 @@
       <c r="J64" t="b">
         <v>1</v>
       </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2920,6 +3240,11 @@
       <c r="J65" t="b">
         <v>1</v>
       </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2958,6 +3283,11 @@
       <c r="J66" t="b">
         <v>0</v>
       </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3000,6 +3330,11 @@
       <c r="J67" t="b">
         <v>0</v>
       </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3042,6 +3377,11 @@
       <c r="J68" t="b">
         <v>0</v>
       </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3084,6 +3424,11 @@
       <c r="J69" t="b">
         <v>0</v>
       </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3126,6 +3471,11 @@
       <c r="J70" t="b">
         <v>0</v>
       </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>GENETIC</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3164,6 +3514,11 @@
       <c r="J71" t="b">
         <v>1</v>
       </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3202,6 +3557,11 @@
       <c r="J72" t="b">
         <v>1</v>
       </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3239,6 +3599,11 @@
       </c>
       <c r="J73" t="b">
         <v>0</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -3274,6 +3639,11 @@
       <c r="J74" t="b">
         <v>0</v>
       </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3312,6 +3682,11 @@
       <c r="J75" t="b">
         <v>0</v>
       </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3350,6 +3725,11 @@
       <c r="J76" t="b">
         <v>0</v>
       </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3388,6 +3768,11 @@
       <c r="J77" t="b">
         <v>0</v>
       </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3430,6 +3815,11 @@
       <c r="J78" t="b">
         <v>1</v>
       </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3472,6 +3862,11 @@
       <c r="J79" t="b">
         <v>1</v>
       </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3514,6 +3909,11 @@
       <c r="J80" t="b">
         <v>0</v>
       </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3552,6 +3952,11 @@
       <c r="J81" t="b">
         <v>0</v>
       </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3590,6 +3995,11 @@
       <c r="J82" t="b">
         <v>1</v>
       </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3628,6 +4038,11 @@
       <c r="J83" t="b">
         <v>0</v>
       </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3666,6 +4081,11 @@
       <c r="J84" t="b">
         <v>0</v>
       </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3704,6 +4124,11 @@
       <c r="J85" t="b">
         <v>1</v>
       </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3746,6 +4171,11 @@
       <c r="J86" t="b">
         <v>0</v>
       </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3784,6 +4214,11 @@
       <c r="J87" t="b">
         <v>1</v>
       </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3826,6 +4261,11 @@
       <c r="J88" t="b">
         <v>0</v>
       </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3864,6 +4304,11 @@
       <c r="J89" t="b">
         <v>1</v>
       </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3906,6 +4351,11 @@
       <c r="J90" t="b">
         <v>0</v>
       </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3948,6 +4398,11 @@
       <c r="J91" t="b">
         <v>0</v>
       </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3986,6 +4441,11 @@
       <c r="J92" t="b">
         <v>0</v>
       </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4028,6 +4488,11 @@
       <c r="J93" t="b">
         <v>1</v>
       </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4070,6 +4535,11 @@
       <c r="J94" t="b">
         <v>1</v>
       </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4108,6 +4578,11 @@
       <c r="J95" t="b">
         <v>0</v>
       </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4146,6 +4621,11 @@
       <c r="J96" t="b">
         <v>0</v>
       </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4184,6 +4664,11 @@
       <c r="J97" t="b">
         <v>0</v>
       </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4226,6 +4711,11 @@
       <c r="J98" t="b">
         <v>0</v>
       </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4264,6 +4754,11 @@
       <c r="J99" t="b">
         <v>1</v>
       </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4302,6 +4797,11 @@
       <c r="J100" t="b">
         <v>0</v>
       </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4344,6 +4844,11 @@
       <c r="J101" t="b">
         <v>0</v>
       </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4386,6 +4891,11 @@
       <c r="J102" t="b">
         <v>0</v>
       </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4424,6 +4934,11 @@
       <c r="J103" t="b">
         <v>0</v>
       </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4466,6 +4981,11 @@
       <c r="J104" t="b">
         <v>1</v>
       </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4508,6 +5028,11 @@
       <c r="J105" t="b">
         <v>0</v>
       </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4546,6 +5071,11 @@
       <c r="J106" t="b">
         <v>0</v>
       </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4588,6 +5118,11 @@
       <c r="J107" t="b">
         <v>1</v>
       </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4630,6 +5165,11 @@
       <c r="J108" t="b">
         <v>0</v>
       </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4672,6 +5212,11 @@
       <c r="J109" t="b">
         <v>0</v>
       </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4714,6 +5259,11 @@
       <c r="J110" t="b">
         <v>0</v>
       </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4756,6 +5306,11 @@
       <c r="J111" t="b">
         <v>1</v>
       </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4798,6 +5353,11 @@
       <c r="J112" t="b">
         <v>0</v>
       </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4840,6 +5400,11 @@
       <c r="J113" t="b">
         <v>1</v>
       </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4882,6 +5447,11 @@
       <c r="J114" t="b">
         <v>0</v>
       </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4924,6 +5494,11 @@
       <c r="J115" t="b">
         <v>0</v>
       </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4965,6 +5540,11 @@
       </c>
       <c r="J116" t="b">
         <v>1</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
       </c>
     </row>
     <row r="117">
@@ -5000,6 +5580,11 @@
       <c r="J117" t="b">
         <v>0</v>
       </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5034,6 +5619,11 @@
       <c r="J118" t="b">
         <v>0</v>
       </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5072,6 +5662,11 @@
       <c r="J119" t="b">
         <v>0</v>
       </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5114,6 +5709,11 @@
       <c r="J120" t="b">
         <v>0</v>
       </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5152,6 +5752,11 @@
       <c r="J121" t="b">
         <v>0</v>
       </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5194,6 +5799,11 @@
       <c r="J122" t="b">
         <v>0</v>
       </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5236,6 +5846,11 @@
       <c r="J123" t="b">
         <v>0</v>
       </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5278,6 +5893,11 @@
       <c r="J124" t="b">
         <v>0</v>
       </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5315,6 +5935,11 @@
       </c>
       <c r="J125" t="b">
         <v>0</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
       </c>
     </row>
     <row r="126">
@@ -5350,6 +5975,11 @@
       <c r="J126" t="b">
         <v>0</v>
       </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5392,6 +6022,11 @@
       <c r="J127" t="b">
         <v>1</v>
       </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5434,6 +6069,11 @@
       <c r="J128" t="b">
         <v>0</v>
       </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5476,6 +6116,11 @@
       <c r="J129" t="b">
         <v>1</v>
       </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5514,6 +6159,11 @@
       <c r="J130" t="b">
         <v>0</v>
       </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5556,6 +6206,11 @@
       <c r="J131" t="b">
         <v>1</v>
       </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5598,6 +6253,11 @@
       <c r="J132" t="b">
         <v>0</v>
       </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5636,6 +6296,11 @@
       <c r="J133" t="b">
         <v>0</v>
       </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5674,6 +6339,11 @@
       <c r="J134" t="b">
         <v>0</v>
       </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5712,6 +6382,11 @@
       <c r="J135" t="b">
         <v>0</v>
       </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5754,6 +6429,11 @@
       <c r="J136" t="b">
         <v>1</v>
       </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5792,6 +6472,11 @@
       <c r="J137" t="b">
         <v>0</v>
       </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5834,6 +6519,11 @@
       <c r="J138" t="b">
         <v>0</v>
       </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>GENETIC</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5876,6 +6566,11 @@
       <c r="J139" t="b">
         <v>0</v>
       </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5918,6 +6613,11 @@
       <c r="J140" t="b">
         <v>0</v>
       </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5956,6 +6656,11 @@
       <c r="J141" t="b">
         <v>1</v>
       </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5998,6 +6703,11 @@
       <c r="J142" t="b">
         <v>0</v>
       </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -6036,6 +6746,11 @@
       <c r="J143" t="b">
         <v>0</v>
       </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -6078,6 +6793,11 @@
       <c r="J144" t="b">
         <v>0</v>
       </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -6120,6 +6840,11 @@
       <c r="J145" t="b">
         <v>0</v>
       </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -6157,6 +6882,11 @@
       </c>
       <c r="J146" t="b">
         <v>0</v>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
       </c>
     </row>
     <row r="147">
@@ -6192,6 +6922,11 @@
       <c r="J147" t="b">
         <v>0</v>
       </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -6229,6 +6964,11 @@
       </c>
       <c r="J148" t="b">
         <v>0</v>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
       </c>
     </row>
     <row r="149">
@@ -6264,6 +7004,11 @@
       <c r="J149" t="b">
         <v>0</v>
       </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6302,6 +7047,11 @@
       <c r="J150" t="b">
         <v>0</v>
       </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6340,6 +7090,11 @@
       <c r="J151" t="b">
         <v>0</v>
       </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -6382,6 +7137,11 @@
       <c r="J152" t="b">
         <v>0</v>
       </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -6420,6 +7180,11 @@
       <c r="J153" t="b">
         <v>0</v>
       </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -6458,6 +7223,11 @@
       <c r="J154" t="b">
         <v>0</v>
       </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -6496,6 +7266,11 @@
       <c r="J155" t="b">
         <v>0</v>
       </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -6538,6 +7313,11 @@
       <c r="J156" t="b">
         <v>0</v>
       </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -6576,6 +7356,11 @@
       <c r="J157" t="b">
         <v>0</v>
       </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>GENETIC</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -6618,6 +7403,11 @@
       <c r="J158" t="b">
         <v>0</v>
       </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -6656,6 +7446,11 @@
       <c r="J159" t="b">
         <v>0</v>
       </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -6698,6 +7493,11 @@
       <c r="J160" t="b">
         <v>1</v>
       </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -6736,6 +7536,11 @@
       <c r="J161" t="b">
         <v>0</v>
       </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -6778,6 +7583,11 @@
       <c r="J162" t="b">
         <v>0</v>
       </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -6816,6 +7626,11 @@
       <c r="J163" t="b">
         <v>0</v>
       </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -6854,6 +7669,11 @@
       <c r="J164" t="b">
         <v>0</v>
       </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -6892,6 +7712,11 @@
       <c r="J165" t="b">
         <v>0</v>
       </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -6934,6 +7759,11 @@
       <c r="J166" t="b">
         <v>1</v>
       </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -6976,6 +7806,11 @@
       <c r="J167" t="b">
         <v>0</v>
       </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -7018,6 +7853,11 @@
       <c r="J168" t="b">
         <v>0</v>
       </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -7056,6 +7896,11 @@
       <c r="J169" t="b">
         <v>0</v>
       </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -7098,6 +7943,11 @@
       <c r="J170" t="b">
         <v>0</v>
       </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -7135,6 +7985,11 @@
       </c>
       <c r="J171" t="b">
         <v>0</v>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>RADIATION</t>
+        </is>
       </c>
     </row>
     <row r="172">
@@ -7170,6 +8025,11 @@
       <c r="J172" t="b">
         <v>0</v>
       </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -7212,6 +8072,11 @@
       <c r="J173" t="b">
         <v>0</v>
       </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -7250,6 +8115,11 @@
       <c r="J174" t="b">
         <v>0</v>
       </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -7292,6 +8162,11 @@
       <c r="J175" t="b">
         <v>0</v>
       </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -7330,6 +8205,11 @@
       <c r="J176" t="b">
         <v>0</v>
       </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -7372,6 +8252,11 @@
       <c r="J177" t="b">
         <v>0</v>
       </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -7414,6 +8299,11 @@
       <c r="J178" t="b">
         <v>0</v>
       </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -7452,6 +8342,11 @@
       <c r="J179" t="b">
         <v>0</v>
       </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -7493,6 +8388,11 @@
       </c>
       <c r="J180" t="b">
         <v>0</v>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
       </c>
     </row>
     <row r="181">
@@ -7528,6 +8428,11 @@
       <c r="J181" t="b">
         <v>0</v>
       </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -7566,6 +8471,11 @@
       <c r="J182" t="b">
         <v>0</v>
       </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -7608,6 +8518,11 @@
       <c r="J183" t="b">
         <v>0</v>
       </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -7650,6 +8565,11 @@
       <c r="J184" t="b">
         <v>0</v>
       </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -7692,6 +8612,11 @@
       <c r="J185" t="b">
         <v>0</v>
       </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -7730,6 +8655,11 @@
       <c r="J186" t="b">
         <v>0</v>
       </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -7772,6 +8702,11 @@
       <c r="J187" t="b">
         <v>1</v>
       </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -7814,6 +8749,11 @@
       <c r="J188" t="b">
         <v>0</v>
       </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -7852,6 +8792,11 @@
       <c r="J189" t="b">
         <v>1</v>
       </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -7890,6 +8835,11 @@
       <c r="J190" t="b">
         <v>0</v>
       </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -7932,6 +8882,11 @@
       <c r="J191" t="b">
         <v>1</v>
       </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -7970,6 +8925,11 @@
       <c r="J192" t="b">
         <v>1</v>
       </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -8012,6 +8972,11 @@
       <c r="J193" t="b">
         <v>0</v>
       </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -8050,6 +9015,11 @@
       <c r="J194" t="b">
         <v>1</v>
       </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -8092,6 +9062,11 @@
       <c r="J195" t="b">
         <v>0</v>
       </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -8134,6 +9109,11 @@
       <c r="J196" t="b">
         <v>0</v>
       </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -8172,6 +9152,11 @@
       <c r="J197" t="b">
         <v>0</v>
       </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -8214,6 +9199,11 @@
       <c r="J198" t="b">
         <v>0</v>
       </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>DIAGNOSTIC_TEST</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -8256,6 +9246,11 @@
       <c r="J199" t="b">
         <v>0</v>
       </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -8298,6 +9293,11 @@
       <c r="J200" t="b">
         <v>0</v>
       </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -8340,6 +9340,11 @@
       <c r="J201" t="b">
         <v>0</v>
       </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>DEVICE</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -8381,6 +9386,11 @@
       </c>
       <c r="J202" t="b">
         <v>0</v>
+      </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
       </c>
     </row>
     <row r="203">
@@ -8416,6 +9426,11 @@
       <c r="J203" t="b">
         <v>1</v>
       </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>DRUG</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -8450,6 +9465,11 @@
       <c r="J204" t="b">
         <v>0</v>
       </c>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -8484,6 +9504,11 @@
       <c r="J205" t="b">
         <v>0</v>
       </c>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -8518,6 +9543,11 @@
       <c r="J206" t="b">
         <v>1</v>
       </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -8552,6 +9582,11 @@
       <c r="J207" t="b">
         <v>0</v>
       </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>BIOLOGICAL</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -8586,6 +9621,11 @@
       <c r="J208" t="b">
         <v>0</v>
       </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -8620,6 +9660,11 @@
       <c r="J209" t="b">
         <v>0</v>
       </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -8654,6 +9699,11 @@
       <c r="J210" t="b">
         <v>1</v>
       </c>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -8688,6 +9738,11 @@
       <c r="J211" t="b">
         <v>0</v>
       </c>
+      <c r="K211" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -8722,6 +9777,11 @@
       <c r="J212" t="b">
         <v>1</v>
       </c>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>PROCEDURE</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -8760,6 +9820,11 @@
       <c r="J213" t="b">
         <v>0</v>
       </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>BEHAVIORAL</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -8793,6 +9858,11 @@
       </c>
       <c r="J214" t="b">
         <v>0</v>
+      </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>